<commit_message>
stats for different efficiency
</commit_message>
<xml_diff>
--- a/user_files/Valetta6789_stats.xlsx
+++ b/user_files/Valetta6789_stats.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="13" uniqueCount="8">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="75" uniqueCount="13">
   <si>
     <t>Count</t>
   </si>
@@ -38,6 +38,21 @@
   </si>
   <si>
     <t>%</t>
+  </si>
+  <si>
+    <t>Totals</t>
+  </si>
+  <si>
+    <t>Easy</t>
+  </si>
+  <si>
+    <t>Single dark</t>
+  </si>
+  <si>
+    <t>Easy null</t>
+  </si>
+  <si>
+    <t>Double dark</t>
   </si>
 </sst>
 </file>
@@ -414,119 +429,576 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:D8"/>
+  <dimension ref="A1:D49"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <sheetData>
     <row r="1" spans="1:4">
-      <c r="A1" s="1" t="s">
+      <c r="A1" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4">
+      <c r="A2" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="1" t="s">
+      <c r="B2" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="1" t="s">
+      <c r="C2" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="1" t="s">
+      <c r="D2" s="1" t="s">
         <v>3</v>
-      </c>
-    </row>
-    <row r="2" spans="1:4">
-      <c r="A2" t="s">
-        <v>4</v>
-      </c>
-      <c r="B2">
-        <v>644</v>
-      </c>
-      <c r="C2">
-        <v>537</v>
-      </c>
-      <c r="D2">
-        <v>1181</v>
       </c>
     </row>
     <row r="3" spans="1:4">
       <c r="A3" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="B3">
-        <v>2941</v>
+        <v>644</v>
       </c>
       <c r="C3">
-        <v>2361</v>
+        <v>537</v>
       </c>
       <c r="D3">
-        <v>5302</v>
+        <v>1181</v>
       </c>
     </row>
     <row r="4" spans="1:4">
       <c r="A4" t="s">
+        <v>5</v>
+      </c>
+      <c r="B4">
+        <v>2941</v>
+      </c>
+      <c r="C4">
+        <v>2361</v>
+      </c>
+      <c r="D4">
+        <v>5302</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4">
+      <c r="A5" t="s">
         <v>6</v>
       </c>
-      <c r="B4">
+      <c r="B5">
         <v>3585</v>
       </c>
-      <c r="C4">
+      <c r="C5">
         <v>2898</v>
       </c>
-      <c r="D4">
+      <c r="D5">
         <v>6483</v>
       </c>
     </row>
-    <row r="6" spans="1:4">
-      <c r="A6" s="1" t="s">
+    <row r="7" spans="1:4">
+      <c r="A7" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="B6" s="1" t="s">
+      <c r="B7" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="C6" s="1" t="s">
+      <c r="C7" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="D6" s="1" t="s">
+      <c r="D7" s="1" t="s">
         <v>3</v>
-      </c>
-    </row>
-    <row r="7" spans="1:4">
-      <c r="A7" t="s">
-        <v>4</v>
-      </c>
-      <c r="B7">
-        <v>17.96</v>
-      </c>
-      <c r="C7">
-        <v>18.53</v>
-      </c>
-      <c r="D7">
-        <v>18.22</v>
       </c>
     </row>
     <row r="8" spans="1:4">
       <c r="A8" t="s">
+        <v>4</v>
+      </c>
+      <c r="B8">
+        <v>17.96</v>
+      </c>
+      <c r="C8">
+        <v>18.53</v>
+      </c>
+      <c r="D8">
+        <v>18.22</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4">
+      <c r="A9" t="s">
         <v>5</v>
       </c>
-      <c r="B8">
+      <c r="B9">
         <v>82.04000000000001</v>
       </c>
-      <c r="C8">
+      <c r="C9">
         <v>81.47</v>
       </c>
-      <c r="D8">
+      <c r="D9">
         <v>81.78</v>
       </c>
     </row>
+    <row r="11" spans="1:4">
+      <c r="A11" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="12" spans="1:4">
+      <c r="A12" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B12" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C12" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D12" s="1" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="13" spans="1:4">
+      <c r="A13" t="s">
+        <v>4</v>
+      </c>
+      <c r="B13">
+        <v>441</v>
+      </c>
+      <c r="C13">
+        <v>399</v>
+      </c>
+      <c r="D13">
+        <v>840</v>
+      </c>
+    </row>
+    <row r="14" spans="1:4">
+      <c r="A14" t="s">
+        <v>5</v>
+      </c>
+      <c r="B14">
+        <v>1169</v>
+      </c>
+      <c r="C14">
+        <v>1443</v>
+      </c>
+      <c r="D14">
+        <v>2612</v>
+      </c>
+    </row>
+    <row r="15" spans="1:4">
+      <c r="A15" t="s">
+        <v>6</v>
+      </c>
+      <c r="B15">
+        <v>1610</v>
+      </c>
+      <c r="C15">
+        <v>1842</v>
+      </c>
+      <c r="D15">
+        <v>3452</v>
+      </c>
+    </row>
+    <row r="17" spans="1:4">
+      <c r="A17" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="B17" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C17" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D17" s="1" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="18" spans="1:4">
+      <c r="A18" t="s">
+        <v>4</v>
+      </c>
+      <c r="B18">
+        <v>27.39</v>
+      </c>
+      <c r="C18">
+        <v>21.66</v>
+      </c>
+      <c r="D18">
+        <v>24.33</v>
+      </c>
+    </row>
+    <row r="19" spans="1:4">
+      <c r="A19" t="s">
+        <v>5</v>
+      </c>
+      <c r="B19">
+        <v>72.61</v>
+      </c>
+      <c r="C19">
+        <v>78.34</v>
+      </c>
+      <c r="D19">
+        <v>75.67</v>
+      </c>
+    </row>
+    <row r="21" spans="1:4">
+      <c r="A21" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="22" spans="1:4">
+      <c r="A22" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B22" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C22" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D22" s="1" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="23" spans="1:4">
+      <c r="A23" t="s">
+        <v>4</v>
+      </c>
+      <c r="B23">
+        <v>181</v>
+      </c>
+      <c r="C23">
+        <v>114</v>
+      </c>
+      <c r="D23">
+        <v>295</v>
+      </c>
+    </row>
+    <row r="24" spans="1:4">
+      <c r="A24" t="s">
+        <v>5</v>
+      </c>
+      <c r="B24">
+        <v>1448</v>
+      </c>
+      <c r="C24">
+        <v>761</v>
+      </c>
+      <c r="D24">
+        <v>2209</v>
+      </c>
+    </row>
+    <row r="25" spans="1:4">
+      <c r="A25" t="s">
+        <v>6</v>
+      </c>
+      <c r="B25">
+        <v>1629</v>
+      </c>
+      <c r="C25">
+        <v>875</v>
+      </c>
+      <c r="D25">
+        <v>2504</v>
+      </c>
+    </row>
+    <row r="27" spans="1:4">
+      <c r="A27" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="B27" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C27" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D27" s="1" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="28" spans="1:4">
+      <c r="A28" t="s">
+        <v>4</v>
+      </c>
+      <c r="B28">
+        <v>11.11</v>
+      </c>
+      <c r="C28">
+        <v>13.03</v>
+      </c>
+      <c r="D28">
+        <v>11.78</v>
+      </c>
+    </row>
+    <row r="29" spans="1:4">
+      <c r="A29" t="s">
+        <v>5</v>
+      </c>
+      <c r="B29">
+        <v>88.89</v>
+      </c>
+      <c r="C29">
+        <v>86.97</v>
+      </c>
+      <c r="D29">
+        <v>88.22</v>
+      </c>
+    </row>
+    <row r="31" spans="1:4">
+      <c r="A31" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="32" spans="1:4">
+      <c r="A32" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B32" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C32" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D32" s="1" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="33" spans="1:4">
+      <c r="A33" t="s">
+        <v>4</v>
+      </c>
+      <c r="B33">
+        <v>13</v>
+      </c>
+      <c r="C33">
+        <v>23</v>
+      </c>
+      <c r="D33">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="34" spans="1:4">
+      <c r="A34" t="s">
+        <v>5</v>
+      </c>
+      <c r="B34">
+        <v>50</v>
+      </c>
+      <c r="C34">
+        <v>96</v>
+      </c>
+      <c r="D34">
+        <v>146</v>
+      </c>
+    </row>
+    <row r="35" spans="1:4">
+      <c r="A35" t="s">
+        <v>6</v>
+      </c>
+      <c r="B35">
+        <v>63</v>
+      </c>
+      <c r="C35">
+        <v>119</v>
+      </c>
+      <c r="D35">
+        <v>182</v>
+      </c>
+    </row>
+    <row r="37" spans="1:4">
+      <c r="A37" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="B37" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C37" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D37" s="1" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="38" spans="1:4">
+      <c r="A38" t="s">
+        <v>4</v>
+      </c>
+      <c r="B38">
+        <v>20.63</v>
+      </c>
+      <c r="C38">
+        <v>19.33</v>
+      </c>
+      <c r="D38">
+        <v>19.78</v>
+      </c>
+    </row>
+    <row r="39" spans="1:4">
+      <c r="A39" t="s">
+        <v>5</v>
+      </c>
+      <c r="B39">
+        <v>79.37</v>
+      </c>
+      <c r="C39">
+        <v>80.67</v>
+      </c>
+      <c r="D39">
+        <v>80.22</v>
+      </c>
+    </row>
+    <row r="41" spans="1:4">
+      <c r="A41" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="42" spans="1:4">
+      <c r="A42" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B42" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C42" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D42" s="1" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="43" spans="1:4">
+      <c r="A43" t="s">
+        <v>4</v>
+      </c>
+      <c r="B43">
+        <v>9</v>
+      </c>
+      <c r="C43">
+        <v>1</v>
+      </c>
+      <c r="D43">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="44" spans="1:4">
+      <c r="A44" t="s">
+        <v>5</v>
+      </c>
+      <c r="B44">
+        <v>274</v>
+      </c>
+      <c r="C44">
+        <v>61</v>
+      </c>
+      <c r="D44">
+        <v>335</v>
+      </c>
+    </row>
+    <row r="45" spans="1:4">
+      <c r="A45" t="s">
+        <v>6</v>
+      </c>
+      <c r="B45">
+        <v>283</v>
+      </c>
+      <c r="C45">
+        <v>62</v>
+      </c>
+      <c r="D45">
+        <v>345</v>
+      </c>
+    </row>
+    <row r="47" spans="1:4">
+      <c r="A47" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="B47" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C47" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D47" s="1" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="48" spans="1:4">
+      <c r="A48" t="s">
+        <v>4</v>
+      </c>
+      <c r="B48">
+        <v>3.18</v>
+      </c>
+      <c r="C48">
+        <v>1.61</v>
+      </c>
+      <c r="D48">
+        <v>2.9</v>
+      </c>
+    </row>
+    <row r="49" spans="1:4">
+      <c r="A49" t="s">
+        <v>5</v>
+      </c>
+      <c r="B49">
+        <v>96.81999999999999</v>
+      </c>
+      <c r="C49">
+        <v>98.39</v>
+      </c>
+      <c r="D49">
+        <v>97.09999999999999</v>
+      </c>
+    </row>
   </sheetData>
-  <conditionalFormatting sqref="A1:D4">
-    <cfRule type="notContainsErrors" dxfId="0" priority="1">
-      <formula>NOT(ISERROR(A1))</formula>
+  <conditionalFormatting sqref="A12:D15">
+    <cfRule type="notContainsErrors" dxfId="0" priority="3">
+      <formula>NOT(ISERROR(A12))</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="A6:D8">
+  <conditionalFormatting sqref="A17:D19">
+    <cfRule type="notContainsErrors" dxfId="0" priority="4">
+      <formula>NOT(ISERROR(A17))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="A22:D25">
+    <cfRule type="notContainsErrors" dxfId="0" priority="5">
+      <formula>NOT(ISERROR(A22))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="A27:D29">
+    <cfRule type="notContainsErrors" dxfId="0" priority="6">
+      <formula>NOT(ISERROR(A27))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="A2:D5">
+    <cfRule type="notContainsErrors" dxfId="0" priority="1">
+      <formula>NOT(ISERROR(A2))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="A32:D35">
+    <cfRule type="notContainsErrors" dxfId="0" priority="7">
+      <formula>NOT(ISERROR(A32))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="A37:D39">
+    <cfRule type="notContainsErrors" dxfId="0" priority="8">
+      <formula>NOT(ISERROR(A37))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="A42:D45">
+    <cfRule type="notContainsErrors" dxfId="0" priority="9">
+      <formula>NOT(ISERROR(A42))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="A47:D49">
+    <cfRule type="notContainsErrors" dxfId="0" priority="10">
+      <formula>NOT(ISERROR(A47))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="A7:D9">
     <cfRule type="notContainsErrors" dxfId="0" priority="2">
-      <formula>NOT(ISERROR(A6))</formula>
+      <formula>NOT(ISERROR(A7))</formula>
     </cfRule>
   </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>